<commit_message>
Hyperlink strip down 2
</commit_message>
<xml_diff>
--- a/Sandbox.OpenXML/HyperlinkExample.xlsx
+++ b/Sandbox.OpenXML/HyperlinkExample.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+<x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet name="Hyperlink" sheetId="1" r:id="rId1"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hyperlink" sheetId="1" r:id="rId1"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -77,19 +77,19 @@
 </file>
 
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:cols>
     <x:col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <x:row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" spans="1:1" x14ac:dyDescent="0.35">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="A1" r:id="rId1"/>
+    <x:hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A1" r:id="rId1"/>
   </x:hyperlinks>
 </x:worksheet>
 </file>
</xml_diff>